<commit_message>
Final Working Core functionality of XML/XSD to CSV Conversion Feb 15th 2020
</commit_message>
<xml_diff>
--- a/FI_Activity_Tracker.xlsx
+++ b/FI_Activity_Tracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B455B59-ECFA-4E71-BE0D-566F8B9B1319}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FA8788-D8D6-4B41-8252-688B2A88A42A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -111,6 +111,42 @@
 Incorporated DFS Traversal of nodes, and successfully generated a dynamic sequence of interlinked parent-child nodes in JS.
 Nested hierarchy on selection generates array in JS. Managed to pass this array into server-side Python script and write into csv file.
 Need to implement similar logic for XSD but with more enhancements.</t>
+  </si>
+  <si>
+    <t>Create nested XSD Tags as hierarchical Checkboxes</t>
+  </si>
+  <si>
+    <r>
+      <t>Tried to modify the DFS approach to filter out non-</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">element </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tags</t>
+    </r>
+  </si>
+  <si>
+    <t>Nested XSD Tags &amp; Final Dataframe writing to CSV</t>
+  </si>
+  <si>
+    <t>Successfully displayed nested hierarchical set of XSD Tags.
+Worked on creating final dataframe logic and successfully managed to create Pyspark config.csv file as per discussion with Pooja.</t>
   </si>
 </sst>
 </file>
@@ -120,7 +156,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +174,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -229,7 +273,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -271,6 +315,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -587,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -597,7 +644,7 @@
     <col min="2" max="2" width="10.453125" style="3" customWidth="1"/>
     <col min="3" max="3" width="32.1796875" style="14" customWidth="1"/>
     <col min="4" max="4" width="63.453125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="14.08984375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="14.08984375" style="2" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="23.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -628,13 +675,13 @@
       <c r="B2" s="9">
         <v>0</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="24">
         <v>0.4</v>
       </c>
       <c r="F2" s="9">
@@ -648,9 +695,9 @@
       <c r="B3" s="9">
         <v>1</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="24"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="25"/>
       <c r="F3" s="9">
         <v>8</v>
       </c>
@@ -659,10 +706,10 @@
       <c r="A4" s="8">
         <v>43860</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="26">
         <v>2</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="27" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="10" t="s">
@@ -679,8 +726,8 @@
       <c r="A5" s="8">
         <v>43861</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="26"/>
+      <c r="B5" s="26"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="10" t="s">
         <v>12</v>
       </c>
@@ -695,10 +742,10 @@
       <c r="A6" s="15">
         <v>43862</v>
       </c>
-      <c r="B6" s="25">
+      <c r="B6" s="26">
         <v>3</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="27" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="10" t="s">
@@ -715,8 +762,8 @@
       <c r="A7" s="15">
         <v>43863</v>
       </c>
-      <c r="B7" s="25"/>
-      <c r="C7" s="26"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="27"/>
       <c r="D7" s="10" t="s">
         <v>11</v>
       </c>
@@ -788,7 +835,7 @@
       <c r="B11" s="9">
         <v>7</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="17" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="10" t="s">
@@ -808,7 +855,7 @@
       <c r="B12" s="9">
         <v>8</v>
       </c>
-      <c r="C12" s="17"/>
+      <c r="C12" s="18"/>
       <c r="D12" s="10" t="s">
         <v>17</v>
       </c>
@@ -826,7 +873,7 @@
       <c r="B13" s="9">
         <v>9</v>
       </c>
-      <c r="C13" s="17"/>
+      <c r="C13" s="18"/>
       <c r="D13" s="10" t="s">
         <v>19</v>
       </c>
@@ -844,7 +891,7 @@
       <c r="B14" s="9">
         <v>10</v>
       </c>
-      <c r="C14" s="18"/>
+      <c r="C14" s="19"/>
       <c r="D14" s="10" t="s">
         <v>18</v>
       </c>
@@ -897,41 +944,77 @@
       <c r="A17" s="8">
         <v>43873</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="10"/>
+      <c r="B17" s="9">
+        <v>13</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="E17" s="10"/>
-      <c r="F17" s="12"/>
+      <c r="F17" s="12">
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="8">
         <v>43874</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="10"/>
+      <c r="B18" s="9">
+        <v>14</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>13</v>
+      </c>
       <c r="E18" s="10"/>
-      <c r="F18" s="12"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F18" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="8">
         <v>43875</v>
       </c>
-      <c r="B19" s="9"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="12"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="8">
+      <c r="B19" s="9">
+        <v>15</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="11">
+        <v>0.1</v>
+      </c>
+      <c r="F19" s="12">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="15">
         <v>43876</v>
       </c>
-      <c r="B20" s="9"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="12"/>
+      <c r="B20" s="9">
+        <v>16</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E20" s="11">
+        <v>0.7</v>
+      </c>
+      <c r="F20" s="12">
+        <v>6</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="8">

</xml_diff>